<commit_message>
cleaning up and BOM update
</commit_message>
<xml_diff>
--- a/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-3.xlsx
+++ b/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-3.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenadachi/Documents/GitHub/pufferfish-electronics/designs/Pufferfish-Interface-2/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC0B046-7052-BE4F-A3FD-1BDBBA3E08E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972A4EA0-0D3A-5E4A-A178-9463C486CE94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="460" windowWidth="24000" windowHeight="14500" xr2:uid="{BF342C2E-30CB-B64F-8C68-8C3D8463BC82}"/>
+    <workbookView xWindow="2160" yWindow="460" windowWidth="24000" windowHeight="14500" activeTab="1" xr2:uid="{BF342C2E-30CB-B64F-8C68-8C3D8463BC82}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM (using 2.54mm J2)" sheetId="1" r:id="rId1"/>
-    <sheet name="What we have at Brown" sheetId="3" r:id="rId2"/>
-    <sheet name="BOM (1mm - not finished)" sheetId="2" r:id="rId3"/>
+    <sheet name="Assembly (at Brown)" sheetId="4" r:id="rId2"/>
+    <sheet name="What we have at Brown" sheetId="3" r:id="rId3"/>
+    <sheet name="BOM (1mm - not finished)" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="211">
   <si>
     <t>Image</t>
   </si>
@@ -641,6 +642,33 @@
   </si>
   <si>
     <t>Cart: https://www.digikey.com/short/zfn4zf</t>
+  </si>
+  <si>
+    <t>Move label</t>
+  </si>
+  <si>
+    <t>34,36</t>
+  </si>
+  <si>
+    <t>15-18,28,43</t>
+  </si>
+  <si>
+    <t>3,4,5,6,7,11</t>
+  </si>
+  <si>
+    <t>1-4,8-10,18</t>
+  </si>
+  <si>
+    <t>MISSING</t>
+  </si>
+  <si>
+    <t>5,6,7</t>
+  </si>
+  <si>
+    <t>1-14, 19-27,31, 39-42, 44-45, 47-50</t>
+  </si>
+  <si>
+    <t>1,2,10</t>
   </si>
 </sst>
 </file>
@@ -755,7 +783,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -796,6 +824,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1114,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F16B33-8865-344C-80E0-82EC78AACF85}">
   <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView zoomScale="89" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2189,11 +2226,1724 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB8D72A-3240-714A-8FB7-32F3483C64DF}">
+  <dimension ref="A1:N66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="25"/>
+    <col min="4" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="3">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="8">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <f>H2*4</f>
+        <v>4</v>
+      </c>
+      <c r="J2" s="3">
+        <f>I2-F2</f>
+        <v>2</v>
+      </c>
+      <c r="K2" s="25">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" s="7">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" ref="I3:I38" si="0">H3*4</f>
+        <v>4</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J39" si="1">I3-F3</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="25">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3">
+        <v>30</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H4" s="10">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="K4" s="25">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K5" s="25">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="10">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K6" s="25">
+        <v>8</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="10">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K7" s="25">
+        <v>4</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3">
+        <f>18+10</f>
+        <v>28</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="1"/>
+        <v>-24</v>
+      </c>
+      <c r="K8" s="25">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="10">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K9" s="25">
+        <v>4</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D10" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K10" s="25">
+        <v>3</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M10" s="24" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="3">
+        <v>16</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="8">
+        <v>3</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="K11" s="25">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3">
+        <v>35</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H12" s="8">
+        <v>6</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="1"/>
+        <v>-11</v>
+      </c>
+      <c r="K12" s="25">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="D13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="8">
+        <v>2</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K13" s="25">
+        <v>8</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="30">
+        <v>22272131</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="8">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3">
+        <f>H14*4</f>
+        <v>4</v>
+      </c>
+      <c r="J14" s="3">
+        <f>I14-F14</f>
+        <v>4</v>
+      </c>
+      <c r="K14" s="25">
+        <v>4</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M14" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="27">
+        <v>1718560009</v>
+      </c>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28">
+        <v>2</v>
+      </c>
+      <c r="G15" s="29"/>
+      <c r="H15" s="8">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3">
+        <f>H15*4</f>
+        <v>4</v>
+      </c>
+      <c r="J15" s="3">
+        <f>I15-F15</f>
+        <v>2</v>
+      </c>
+      <c r="K15" s="25">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="8">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K16" s="25">
+        <v>4</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="3">
+        <f>14+5</f>
+        <v>19</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="8">
+        <v>8</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="K17" s="25">
+        <v>13</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="3">
+        <v>4</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="8">
+        <v>3</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J18" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K18" s="25">
+        <v>8</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="8">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K19" s="25">
+        <v>4</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="8">
+        <v>6</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="J20" s="3">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="K20" s="25">
+        <v>24</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="3">
+        <v>100</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H21" s="10">
+        <f>14+9+1+4+2+4</f>
+        <v>34</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="J21" s="3">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="K21" s="25">
+        <v>36</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="32">
+        <v>46</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="14">
+        <v>180</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="10">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K22" s="25">
+        <v>4</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M22" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="14">
+        <v>85</v>
+      </c>
+      <c r="F23" s="3">
+        <v>10</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="H23" s="10">
+        <v>6</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="K23" s="25">
+        <v>14</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="32">
+        <v>29</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="14">
+        <v>820</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="10">
+        <v>1</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K24" s="25">
+        <f>J24</f>
+        <v>4</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M24" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="N24" s="3"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="32">
+        <v>30</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="10">
+        <v>1</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K25" s="25">
+        <f t="shared" ref="K25:K31" si="2">J25</f>
+        <v>4</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="N25" s="3"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="32">
+        <v>32</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="10">
+        <v>1</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J26" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K26" s="25">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M26" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="N26" s="3"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="10">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J27" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K27" s="25">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M27" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="N27" s="3"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="32">
+        <v>35</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="10">
+        <v>1</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J28" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K28" s="25">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M28" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="N28" s="3"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" s="32">
+        <v>37</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J29" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K29" s="25">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="N29" s="3"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C30" s="32">
+        <v>38</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="10">
+        <v>1</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J30" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K30" s="25">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N30" s="3"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="32">
+        <v>33</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="10">
+        <v>1</v>
+      </c>
+      <c r="I31" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J31" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K31" s="25">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N31" s="3"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="3">
+        <v>3</v>
+      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" s="8">
+        <v>1</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J32" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K32" s="25">
+        <v>1</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="N32" s="3"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="32">
+        <v>2</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="10">
+        <v>1</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J33" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K33" s="25">
+        <v>4</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="N33" s="3"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="K34" s="22"/>
+      <c r="M34" s="10"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H35" s="10">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K35" s="22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F36">
+        <v>11</v>
+      </c>
+      <c r="H36" s="10">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>-7</v>
+      </c>
+      <c r="K36" s="22">
+        <v>0</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="H37" s="10">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K37" s="22">
+        <v>0</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="H38" s="10">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="K38" s="22">
+        <v>0</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F39">
+        <v>8</v>
+      </c>
+      <c r="H39" s="10">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <f>H39*4</f>
+        <v>4</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="K39" s="22">
+        <v>0</v>
+      </c>
+      <c r="L39" t="s">
+        <v>174</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M40" s="3"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I41" t="s">
+        <v>201</v>
+      </c>
+      <c r="M41" s="3"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>132</v>
+      </c>
+      <c r="E43" t="s">
+        <v>154</v>
+      </c>
+      <c r="F43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D44" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E44" t="s">
+        <v>155</v>
+      </c>
+      <c r="F44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <v>200</v>
+      </c>
+      <c r="F45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>134</v>
+      </c>
+      <c r="E46" t="s">
+        <v>135</v>
+      </c>
+      <c r="F46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>136</v>
+      </c>
+      <c r="E47" t="s">
+        <v>109</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>137</v>
+      </c>
+      <c r="E48" t="s">
+        <v>138</v>
+      </c>
+      <c r="F48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D49">
+        <v>90160099</v>
+      </c>
+      <c r="E49" t="s">
+        <v>139</v>
+      </c>
+      <c r="F49">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>141</v>
+      </c>
+      <c r="E50" t="s">
+        <v>142</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>143</v>
+      </c>
+      <c r="E51" t="s">
+        <v>144</v>
+      </c>
+      <c r="F51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>146</v>
+      </c>
+      <c r="E52" t="s">
+        <v>145</v>
+      </c>
+      <c r="F52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>147</v>
+      </c>
+      <c r="E53" t="s">
+        <v>148</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>149</v>
+      </c>
+      <c r="E54" t="s">
+        <v>150</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E55" t="s">
+        <v>161</v>
+      </c>
+      <c r="F55">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>50</v>
+      </c>
+      <c r="G56" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="57" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>153</v>
+      </c>
+      <c r="E57" t="s">
+        <v>154</v>
+      </c>
+      <c r="F57">
+        <v>20</v>
+      </c>
+      <c r="G57" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>156</v>
+      </c>
+      <c r="F58">
+        <f>75+20</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>158</v>
+      </c>
+      <c r="E59" t="s">
+        <v>159</v>
+      </c>
+      <c r="F59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>160</v>
+      </c>
+      <c r="E60" t="s">
+        <v>162</v>
+      </c>
+      <c r="F60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <v>22272091</v>
+      </c>
+      <c r="E61" t="s">
+        <v>163</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D62">
+        <v>1718560009</v>
+      </c>
+      <c r="E62" t="s">
+        <v>163</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
+        <v>165</v>
+      </c>
+      <c r="E63" t="s">
+        <v>164</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D64" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="F64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>167</v>
+      </c>
+      <c r="F65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>168</v>
+      </c>
+      <c r="E66" t="s">
+        <v>169</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M17" r:id="rId1" display="https://www.digikey.com/product-detail/en/vishay-siliconix/2N7002E-T1-E3/2N7002E-T1-E3CT-ND/3946142?utm_adgroup=Semiconductor%20Modules&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_RLSA_Buyers&amp;utm_term=&amp;utm_content=Semiconductor%20Modules&amp;gclid=Cj0KCQjwrIf3BRD1ARIsAMuugNtAYg0B4uzN6uG3FDVYlywiEKFAGbXRLO8hnfXG_d9twvCOg1_5j4waAs4CEALw_wcB" xr:uid="{6012C5CB-84AC-8542-A9CB-479663F68E52}"/>
+    <hyperlink ref="M12" r:id="rId2" xr:uid="{F3F64CEA-81BB-4B4E-AF45-237E468D198D}"/>
+    <hyperlink ref="M18" r:id="rId3" display="https://www.digikey.com/product-detail/en/on-semiconductor/FDN337N/FDN337NCT-ND/458950?utm_adgroup=Semiconductor%20Modules&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search&amp;utm_term=&amp;utm_content=Semiconductor%20Modules&amp;gclid=EAIaIQobChMIi9eQ5_aJ6wIViZWzCh0mJgM4EAAYAyAAEgLjm_D_BwE" xr:uid="{CCD9AB93-6BD4-E945-8B3E-DA3B25E60236}"/>
+    <hyperlink ref="M16" r:id="rId4" xr:uid="{6A3550AA-FA07-8B41-A946-F1438ED86523}"/>
+    <hyperlink ref="M19" r:id="rId5" xr:uid="{A049FC51-BD7E-FF4B-BEB1-13A044A2EB62}"/>
+    <hyperlink ref="M20" r:id="rId6" xr:uid="{14A78EEB-2C19-024D-A101-DA8EA65C8898}"/>
+    <hyperlink ref="M32" r:id="rId7" xr:uid="{54B765F6-8036-1B44-B6FF-28FAB147E615}"/>
+    <hyperlink ref="M33" r:id="rId8" xr:uid="{D9D3671B-F9DE-604B-9D97-19E0E4AE91E4}"/>
+    <hyperlink ref="M13" r:id="rId9" xr:uid="{7223F83C-5778-7C4C-A7A5-FA417E8500AC}"/>
+    <hyperlink ref="M38" r:id="rId10" xr:uid="{17529715-0DDA-9343-A8CB-F5469C91BFC1}"/>
+    <hyperlink ref="M39" r:id="rId11" xr:uid="{D78034F5-8187-674C-AF0B-31D91D45CB7E}"/>
+    <hyperlink ref="M37" r:id="rId12" xr:uid="{232FE498-8037-6542-9E9E-06647CC6D73C}"/>
+    <hyperlink ref="M3" r:id="rId13" xr:uid="{0FCF8082-F2A0-6D48-8E40-06241C6AE5C7}"/>
+    <hyperlink ref="M11" r:id="rId14" xr:uid="{2EF30FA9-9F83-3A49-9EDC-81CD4ED7CCDF}"/>
+    <hyperlink ref="M36" r:id="rId15" xr:uid="{DABDF4B4-E70C-3A4E-B1AC-0C8568F61D08}"/>
+    <hyperlink ref="M29" r:id="rId16" xr:uid="{94B2C4E4-F837-F043-83E3-C094982234F2}"/>
+    <hyperlink ref="M30" r:id="rId17" xr:uid="{412D37B6-DFFA-4C40-8532-7A3F72A8EFD7}"/>
+    <hyperlink ref="M31" r:id="rId18" xr:uid="{F49263AE-1D80-764D-ADE7-8A0BC57B6DFC}"/>
+    <hyperlink ref="M4" r:id="rId19" xr:uid="{5CF2DE80-63C2-2142-8955-9EDB10CDDBE6}"/>
+    <hyperlink ref="M5" r:id="rId20" xr:uid="{E2CF836D-BE11-0C4F-8163-222739B0063A}"/>
+    <hyperlink ref="M6" r:id="rId21" xr:uid="{17DFADE9-363F-1842-9A32-EFCF9B826974}"/>
+    <hyperlink ref="M7" r:id="rId22" xr:uid="{F8DD15B0-9FE1-AD4C-9057-7343952E2E7F}"/>
+    <hyperlink ref="M2" r:id="rId23" xr:uid="{03C9053C-3A96-DF4B-ABFA-3D6BA1128055}"/>
+    <hyperlink ref="M9" r:id="rId24" xr:uid="{CC681CFB-8202-3847-9838-D6AC4665E072}"/>
+    <hyperlink ref="M10" r:id="rId25" xr:uid="{304BDFD2-D25C-C74E-98D7-FA53A1524996}"/>
+    <hyperlink ref="M14" r:id="rId26" xr:uid="{F56090AE-9173-F741-B2A4-0DB23A68DCB0}"/>
+    <hyperlink ref="M22" r:id="rId27" xr:uid="{8AE1FF50-9FBB-3645-B0AD-20F2B5AC3B2A}"/>
+    <hyperlink ref="M24" r:id="rId28" xr:uid="{B1BF6C5B-A6D1-8945-9042-F54245F8426C}"/>
+    <hyperlink ref="M26" r:id="rId29" xr:uid="{5A7A3AF7-FDE3-2B4D-B99E-31AA7BE68064}"/>
+    <hyperlink ref="M27" r:id="rId30" xr:uid="{98304664-F7D7-7245-B6FA-6DA2CBEA68F9}"/>
+    <hyperlink ref="M28" r:id="rId31" xr:uid="{FCA9CABB-8979-E246-A59B-06968ACE96DE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700EBAD9-5F74-724E-B20F-063A5BC601FD}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K39"/>
+    <sheetView topLeftCell="A12" zoomScale="94" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3783,7 +5533,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1243D131-AC88-2841-BA58-5847EC392F6F}">
   <dimension ref="A1:T61"/>
   <sheetViews>

</xml_diff>

<commit_message>
buzzer terminal bug fix
</commit_message>
<xml_diff>
--- a/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-3.xlsx
+++ b/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenadachi/Documents/GitHub/pufferfish-electronics/designs/Pufferfish-Interface-2/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972A4EA0-0D3A-5E4A-A178-9463C486CE94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923D532F-8A2E-0A4E-946B-CAC5E78AD35A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="460" windowWidth="24000" windowHeight="14500" activeTab="1" xr2:uid="{BF342C2E-30CB-B64F-8C68-8C3D8463BC82}"/>
+    <workbookView xWindow="2160" yWindow="460" windowWidth="24000" windowHeight="14500" xr2:uid="{BF342C2E-30CB-B64F-8C68-8C3D8463BC82}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM (using 2.54mm J2)" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="228">
   <si>
     <t>Image</t>
   </si>
@@ -669,6 +669,57 @@
   </si>
   <si>
     <t>1,2,10</t>
+  </si>
+  <si>
+    <t>1658620-4</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/1658620-4/ASC20H-ND/825427</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/A3AAH-2006G/A3AAH-2006G-ND/825905</t>
+  </si>
+  <si>
+    <t>A3AAH-2006G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F Cable to control board </t>
+  </si>
+  <si>
+    <t>F adapter to control board</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>TE Connectivity Passive Product</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>Fairchild Semiconductor</t>
+  </si>
+  <si>
+    <t>Soberton Inc</t>
+  </si>
+  <si>
+    <t>Kemet</t>
+  </si>
+  <si>
+    <t>CUI Devices</t>
+  </si>
+  <si>
+    <t>JST Sales America</t>
+  </si>
+  <si>
+    <t>Inspired LED LLC</t>
+  </si>
+  <si>
+    <t>JR Panel</t>
   </si>
 </sst>
 </file>
@@ -1149,10 +1200,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F16B33-8865-344C-80E0-82EC78AACF85}">
-  <dimension ref="A1:T61"/>
+  <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="89" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1282,7 +1333,9 @@
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>224</v>
+      </c>
       <c r="F4" s="9" t="s">
         <v>83</v>
       </c>
@@ -1313,7 +1366,9 @@
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>223</v>
+      </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
         <v>19</v>
@@ -1338,7 +1393,9 @@
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>223</v>
+      </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
         <v>51</v>
@@ -1363,7 +1420,9 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>223</v>
+      </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10" t="s">
         <v>52</v>
@@ -1388,7 +1447,9 @@
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>223</v>
+      </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10" t="s">
         <v>55</v>
@@ -1440,7 +1501,9 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="F10" s="10" t="s">
         <v>58</v>
       </c>
@@ -1562,7 +1625,7 @@
       </c>
       <c r="I14" s="10"/>
       <c r="K14" s="10"/>
-      <c r="L14" s="23" t="s">
+      <c r="L14" s="6" t="s">
         <v>119</v>
       </c>
       <c r="M14" s="10"/>
@@ -1574,7 +1637,9 @@
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="7" t="s">
+        <v>222</v>
+      </c>
       <c r="F15" s="9" t="s">
         <v>81</v>
       </c>
@@ -1653,7 +1718,9 @@
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="E18" s="7" t="s">
+        <v>221</v>
+      </c>
       <c r="F18" s="9" t="s">
         <v>72</v>
       </c>
@@ -1678,7 +1745,9 @@
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="E19" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="F19" s="9" t="s">
         <v>86</v>
       </c>
@@ -1705,7 +1774,9 @@
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
+      <c r="E20" s="10" t="s">
+        <v>219</v>
+      </c>
       <c r="F20" s="9"/>
       <c r="G20" s="8" t="s">
         <v>38</v>
@@ -1719,7 +1790,7 @@
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
-      <c r="L20" s="6" t="s">
+      <c r="L20" s="23" t="s">
         <v>198</v>
       </c>
       <c r="M20" s="10"/>
@@ -1731,7 +1802,9 @@
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="E21" s="3" t="s">
+        <v>218</v>
+      </c>
       <c r="F21" s="9"/>
       <c r="G21" s="14">
         <v>180</v>
@@ -1744,7 +1817,7 @@
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
-      <c r="L21" s="23" t="s">
+      <c r="L21" s="6" t="s">
         <v>181</v>
       </c>
       <c r="M21" s="10"/>
@@ -1756,7 +1829,9 @@
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
+      <c r="E22" s="3" t="s">
+        <v>217</v>
+      </c>
       <c r="F22" s="9"/>
       <c r="G22" s="14">
         <v>85</v>
@@ -1769,7 +1844,7 @@
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
-      <c r="L22" s="6" t="s">
+      <c r="L22" s="23" t="s">
         <v>199</v>
       </c>
       <c r="M22" s="10"/>
@@ -1781,7 +1856,9 @@
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="E23" s="10" t="s">
+        <v>220</v>
+      </c>
       <c r="F23" s="9"/>
       <c r="G23" s="14">
         <v>820</v>
@@ -1794,7 +1871,7 @@
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
-      <c r="L23" s="23" t="s">
+      <c r="L23" s="6" t="s">
         <v>182</v>
       </c>
       <c r="M23" s="10"/>
@@ -1806,7 +1883,9 @@
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="E24" s="3" t="s">
+        <v>218</v>
+      </c>
       <c r="F24" s="9"/>
       <c r="G24" s="10" t="s">
         <v>111</v>
@@ -1831,7 +1910,9 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+      <c r="E25" s="3" t="s">
+        <v>218</v>
+      </c>
       <c r="F25" s="9"/>
       <c r="G25" s="10" t="s">
         <v>112</v>
@@ -1844,7 +1925,7 @@
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
-      <c r="L25" s="23" t="s">
+      <c r="L25" s="6" t="s">
         <v>184</v>
       </c>
       <c r="M25" s="10"/>
@@ -1856,7 +1937,9 @@
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
+      <c r="E26" s="10" t="s">
+        <v>219</v>
+      </c>
       <c r="F26" s="9"/>
       <c r="G26" s="3" t="s">
         <v>113</v>
@@ -1870,7 +1953,7 @@
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
-      <c r="L26" s="23" t="s">
+      <c r="L26" s="6" t="s">
         <v>185</v>
       </c>
       <c r="M26" s="10"/>
@@ -1882,7 +1965,9 @@
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
+      <c r="E27" s="3" t="s">
+        <v>218</v>
+      </c>
       <c r="F27" s="9"/>
       <c r="G27" s="3" t="s">
         <v>114</v>
@@ -1895,7 +1980,7 @@
       </c>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
-      <c r="L27" s="23" t="s">
+      <c r="L27" s="6" t="s">
         <v>186</v>
       </c>
       <c r="M27" s="10"/>
@@ -1905,6 +1990,9 @@
       <c r="B28" s="7" t="s">
         <v>130</v>
       </c>
+      <c r="E28" s="3" t="s">
+        <v>218</v>
+      </c>
       <c r="G28" s="3" t="s">
         <v>115</v>
       </c>
@@ -1926,7 +2014,9 @@
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
+      <c r="E29" s="3" t="s">
+        <v>217</v>
+      </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10" t="s">
         <v>116</v>
@@ -1945,6 +2035,9 @@
       <c r="A30" s="7"/>
       <c r="B30" s="7" t="s">
         <v>129</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>117</v>
@@ -2033,16 +2126,20 @@
       <c r="M33" s="10"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="10"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="7" t="s">
         <v>107</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
+      <c r="E34" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" s="26" t="s">
+        <v>211</v>
+      </c>
       <c r="G34" s="10" t="s">
-        <v>100</v>
+        <v>216</v>
       </c>
       <c r="H34" s="10">
         <v>1</v>
@@ -2050,7 +2147,9 @@
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
-      <c r="L34"/>
+      <c r="L34" s="4" t="s">
+        <v>212</v>
+      </c>
       <c r="M34" s="10"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -2058,75 +2157,111 @@
       <c r="B35" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>44</v>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>214</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>106</v>
+        <v>215</v>
       </c>
       <c r="H35" s="10">
         <v>1</v>
       </c>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
       <c r="L35" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="M35" s="10"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F36" s="5" t="s">
-        <v>42</v>
+      <c r="E36" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H36" s="10">
         <v>1</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
       <c r="B37" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>225</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H37" s="10">
         <v>1</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>104</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
       <c r="B38" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H38" s="10">
         <v>1</v>
       </c>
-      <c r="L38" s="6" t="s">
-        <v>46</v>
+      <c r="L38" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
+      <c r="B39" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H39" s="10">
+        <v>1</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
@@ -2145,15 +2280,19 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="10"/>
+      <c r="G45" s="26"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="10"/>
+      <c r="G46" s="26"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="10"/>
+      <c r="G47" s="26"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="10"/>
+      <c r="G48" s="4"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="10"/>
@@ -2173,8 +2312,8 @@
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="10"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="10"/>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="10"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="10"/>
@@ -2187,6 +2326,9 @@
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="10"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2199,12 +2341,12 @@
     <hyperlink ref="L31" r:id="rId7" xr:uid="{D33F5AD8-CC67-A844-A1E1-80101524E25E}"/>
     <hyperlink ref="L32" r:id="rId8" xr:uid="{D9215314-7CFE-DA47-A1D7-19390D357925}"/>
     <hyperlink ref="L13" r:id="rId9" xr:uid="{8DDF8875-B190-A444-9A37-221CC26BD403}"/>
-    <hyperlink ref="L37" r:id="rId10" xr:uid="{E7400031-33D6-464F-B914-59B190C14542}"/>
-    <hyperlink ref="L38" r:id="rId11" xr:uid="{BC95EABC-810A-F347-87B6-8A04593322E3}"/>
-    <hyperlink ref="L36" r:id="rId12" xr:uid="{99AA1D84-B976-1149-A280-A8A682182D32}"/>
+    <hyperlink ref="L38" r:id="rId10" xr:uid="{E7400031-33D6-464F-B914-59B190C14542}"/>
+    <hyperlink ref="L39" r:id="rId11" xr:uid="{BC95EABC-810A-F347-87B6-8A04593322E3}"/>
+    <hyperlink ref="L37" r:id="rId12" xr:uid="{99AA1D84-B976-1149-A280-A8A682182D32}"/>
     <hyperlink ref="L4" r:id="rId13" xr:uid="{D83C0BFE-0CE3-8F4A-9E23-4086D9698085}"/>
     <hyperlink ref="L11" r:id="rId14" xr:uid="{E26AD4A0-E476-3E4D-AB87-DA159338A6C9}"/>
-    <hyperlink ref="L35" r:id="rId15" xr:uid="{DECDC59F-921C-6048-AFA3-E200E9D0E522}"/>
+    <hyperlink ref="L36" r:id="rId15" xr:uid="{DECDC59F-921C-6048-AFA3-E200E9D0E522}"/>
     <hyperlink ref="L28" r:id="rId16" xr:uid="{00B6E054-4D31-A749-AD65-1D8827F142AA}"/>
     <hyperlink ref="L29" r:id="rId17" xr:uid="{9105F8E8-FD1B-DF4B-946D-57F5779E8814}"/>
     <hyperlink ref="L30" r:id="rId18" xr:uid="{4F6A886E-AB8D-B642-B33F-E37E5D480EF7}"/>
@@ -2220,6 +2362,10 @@
     <hyperlink ref="L25" r:id="rId28" xr:uid="{97768D06-FF68-2943-9666-3EC4F3E5BC99}"/>
     <hyperlink ref="L26" r:id="rId29" xr:uid="{99353A5A-F5BB-2142-AFB6-B146E4039906}"/>
     <hyperlink ref="L27" r:id="rId30" xr:uid="{36F75D9A-78E2-424B-BE66-86F53642B538}"/>
+    <hyperlink ref="L34" r:id="rId31" xr:uid="{87CBE955-24E4-284A-8C69-592FC3B7AC69}"/>
+    <hyperlink ref="L35" r:id="rId32" xr:uid="{6A594783-0F56-734F-828E-66FFCE91489B}"/>
+    <hyperlink ref="L20" r:id="rId33" xr:uid="{E72DC5DE-778F-344D-BC3E-CEC4F0844D88}"/>
+    <hyperlink ref="L22" r:id="rId34" xr:uid="{98755C1E-CB9E-144D-AD3A-D90CBB928749}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2229,8 +2375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB8D72A-3240-714A-8FB7-32F3483C64DF}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="C25" zoomScale="133" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
before reassigning membrane footprint
</commit_message>
<xml_diff>
--- a/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-3.xlsx
+++ b/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-3.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenadachi/Documents/GitHub/pufferfish-electronics/designs/Pufferfish-Interface-2/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923D532F-8A2E-0A4E-946B-CAC5E78AD35A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16A2F08-96D4-FA40-B0B0-A536FC5EE8B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="460" windowWidth="24000" windowHeight="14500" xr2:uid="{BF342C2E-30CB-B64F-8C68-8C3D8463BC82}"/>
+    <workbookView xWindow="920" yWindow="6340" windowWidth="24000" windowHeight="14500" xr2:uid="{BF342C2E-30CB-B64F-8C68-8C3D8463BC82}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM (using 2.54mm J2)" sheetId="1" r:id="rId1"/>
-    <sheet name="Assembly (at Brown)" sheetId="4" r:id="rId2"/>
-    <sheet name="What we have at Brown" sheetId="3" r:id="rId3"/>
-    <sheet name="BOM (1mm - not finished)" sheetId="2" r:id="rId4"/>
+    <sheet name="BOM v2-4" sheetId="5" r:id="rId1"/>
+    <sheet name="BOM (using 2.54mm J2)" sheetId="1" r:id="rId2"/>
+    <sheet name="Assembly (at Brown)" sheetId="4" r:id="rId3"/>
+    <sheet name="What we have at Brown" sheetId="3" r:id="rId4"/>
+    <sheet name="BOM (1mm - not finished)" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="231">
   <si>
     <t>Image</t>
   </si>
@@ -720,13 +721,22 @@
   </si>
   <si>
     <t>JR Panel</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/0908140920/WM3966CT-ND/2421940</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -806,6 +816,73 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF4F4F4F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -834,7 +911,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -885,6 +962,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1199,11 +1299,1173 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1276498-1E89-8941-B615-C6BB44885BEB}">
+  <dimension ref="A1:T62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="10.83203125" style="36"/>
+    <col min="5" max="5" width="32" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="35"/>
+      <c r="B3" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="39">
+        <v>1</v>
+      </c>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="M3" s="38"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="35"/>
+      <c r="B4" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="38">
+        <v>1</v>
+      </c>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="M4" s="38"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="35"/>
+      <c r="B5" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42" t="s">
+        <v>223</v>
+      </c>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="42">
+        <v>6</v>
+      </c>
+      <c r="I5" s="42">
+        <v>805</v>
+      </c>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="42"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="35"/>
+      <c r="B6" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42" t="s">
+        <v>223</v>
+      </c>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="42">
+        <v>1</v>
+      </c>
+      <c r="I6" s="42">
+        <v>805</v>
+      </c>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="42"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="35"/>
+      <c r="B7" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42" t="s">
+        <v>223</v>
+      </c>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="42">
+        <v>2</v>
+      </c>
+      <c r="I7" s="42">
+        <v>805</v>
+      </c>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="M7" s="42"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="35"/>
+      <c r="B8" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42" t="s">
+        <v>223</v>
+      </c>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="42">
+        <v>1</v>
+      </c>
+      <c r="I8" s="42">
+        <v>805</v>
+      </c>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="M8" s="42"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="35"/>
+      <c r="B9" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="39">
+        <v>1</v>
+      </c>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="M9" s="42"/>
+    </row>
+    <row r="10" spans="1:20" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="50"/>
+      <c r="B10" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="F10" s="52">
+        <v>908140920</v>
+      </c>
+      <c r="G10" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="51">
+        <v>1</v>
+      </c>
+      <c r="J10" s="51" t="s">
+        <v>229</v>
+      </c>
+      <c r="L10" s="54" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="35"/>
+      <c r="B11" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="39">
+        <v>3</v>
+      </c>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="M11" s="42"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="35"/>
+      <c r="B12" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="39">
+        <v>6</v>
+      </c>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="42"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="35"/>
+      <c r="B13" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" s="39">
+        <v>2</v>
+      </c>
+      <c r="I13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="M13" s="42"/>
+    </row>
+    <row r="14" spans="1:20" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="50"/>
+      <c r="B14" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="F14" s="52">
+        <v>526101333</v>
+      </c>
+      <c r="G14" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="53">
+        <v>1</v>
+      </c>
+      <c r="J14" s="51" t="s">
+        <v>229</v>
+      </c>
+      <c r="L14" s="54"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="35"/>
+      <c r="B15" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="38" t="s">
+        <v>222</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="39">
+        <v>1</v>
+      </c>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="M15" s="42"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="35"/>
+      <c r="B16" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="39">
+        <v>8</v>
+      </c>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="42"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="35"/>
+      <c r="B17" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="39">
+        <v>3</v>
+      </c>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="M17" s="42"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="35"/>
+      <c r="B18" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="H18" s="39">
+        <v>1</v>
+      </c>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="M18" s="42"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="35"/>
+      <c r="B19" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="39">
+        <v>6</v>
+      </c>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="M19" s="42"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42" t="s">
+        <v>219</v>
+      </c>
+      <c r="F20" s="41"/>
+      <c r="G20" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="42">
+        <f>14+9+1+4+2+4</f>
+        <v>34</v>
+      </c>
+      <c r="I20" s="36">
+        <v>805</v>
+      </c>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="M20" s="42"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="35"/>
+      <c r="B21" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="F21" s="41"/>
+      <c r="G21" s="45">
+        <v>180</v>
+      </c>
+      <c r="H21" s="42">
+        <v>1</v>
+      </c>
+      <c r="I21" s="36">
+        <v>805</v>
+      </c>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="M21" s="42"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="35"/>
+      <c r="B22" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="F22" s="41"/>
+      <c r="G22" s="45">
+        <v>85</v>
+      </c>
+      <c r="H22" s="42">
+        <v>6</v>
+      </c>
+      <c r="I22" s="36">
+        <v>805</v>
+      </c>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="M22" s="42"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="35"/>
+      <c r="B23" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42" t="s">
+        <v>220</v>
+      </c>
+      <c r="F23" s="41"/>
+      <c r="G23" s="45">
+        <v>820</v>
+      </c>
+      <c r="H23" s="42">
+        <v>1</v>
+      </c>
+      <c r="I23" s="36">
+        <v>805</v>
+      </c>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="M23" s="42"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="35"/>
+      <c r="B24" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="F24" s="41"/>
+      <c r="G24" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="H24" s="42">
+        <v>1</v>
+      </c>
+      <c r="I24" s="36">
+        <v>805</v>
+      </c>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="M24" s="42"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="35"/>
+      <c r="B25" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="F25" s="41"/>
+      <c r="G25" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="42">
+        <v>1</v>
+      </c>
+      <c r="I25" s="36">
+        <v>805</v>
+      </c>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="M25" s="42"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="35"/>
+      <c r="B26" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42" t="s">
+        <v>219</v>
+      </c>
+      <c r="F26" s="41"/>
+      <c r="G26" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="H26" s="42">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+      <c r="I26" s="36">
+        <v>805</v>
+      </c>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="M26" s="42"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="35"/>
+      <c r="B27" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="F27" s="41"/>
+      <c r="G27" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="H27" s="42">
+        <v>1</v>
+      </c>
+      <c r="I27" s="36">
+        <v>805</v>
+      </c>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="M27" s="42"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="35"/>
+      <c r="B28" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="G28" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="H28" s="36">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="36">
+        <v>805</v>
+      </c>
+      <c r="L28" s="37" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="35"/>
+      <c r="B29" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="H29" s="42">
+        <v>1</v>
+      </c>
+      <c r="I29" s="36">
+        <v>805</v>
+      </c>
+      <c r="L29" s="37" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="38"/>
+      <c r="B30" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="E30" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="G30" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="H30" s="42">
+        <v>1</v>
+      </c>
+      <c r="I30" s="36">
+        <v>805</v>
+      </c>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="M30" s="42"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="38"/>
+      <c r="B31" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="G31" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="H31" s="39">
+        <v>1</v>
+      </c>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="M31" s="42"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="42"/>
+      <c r="B32" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="H32" s="42">
+        <v>1</v>
+      </c>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="M32" s="42"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="42"/>
+      <c r="M33" s="42"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="47"/>
+      <c r="B34" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" s="43" t="s">
+        <v>211</v>
+      </c>
+      <c r="G34" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="H34" s="42">
+        <v>1</v>
+      </c>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="M34" s="42"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="42"/>
+      <c r="B35" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="G35" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="H35" s="42">
+        <v>1</v>
+      </c>
+      <c r="I35" s="42"/>
+      <c r="J35" s="42"/>
+      <c r="K35" s="42"/>
+      <c r="L35" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="M35" s="42"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="42"/>
+      <c r="B36" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="E36" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="G36" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="H36" s="42">
+        <v>1</v>
+      </c>
+      <c r="L36" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="42"/>
+      <c r="B37" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="E37" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="F37" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="G37" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="H37" s="42">
+        <v>1</v>
+      </c>
+      <c r="L37" s="37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="42"/>
+      <c r="B38" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="E38" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="F38" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="G38" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="H38" s="42">
+        <v>1</v>
+      </c>
+      <c r="L38" s="37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="42"/>
+      <c r="B39" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="G39" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="H39" s="42">
+        <v>1</v>
+      </c>
+      <c r="L39" s="40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="42"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="42"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="42"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="42"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="42"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="42"/>
+      <c r="G45" s="43"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="42"/>
+      <c r="G46" s="43"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="42"/>
+      <c r="G47" s="43"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="42"/>
+      <c r="G48" s="37"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="42"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="42"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="42"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="42"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="42"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="42"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="42"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="42"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="42"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="42"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="42"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="42"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L16" r:id="rId1" display="https://www.digikey.com/product-detail/en/vishay-siliconix/2N7002E-T1-E3/2N7002E-T1-E3CT-ND/3946142?utm_adgroup=Semiconductor%20Modules&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_RLSA_Buyers&amp;utm_term=&amp;utm_content=Semiconductor%20Modules&amp;gclid=Cj0KCQjwrIf3BRD1ARIsAMuugNtAYg0B4uzN6uG3FDVYlywiEKFAGbXRLO8hnfXG_d9twvCOg1_5j4waAs4CEALw_wcB" xr:uid="{9CE1DA2A-DDC6-0E4A-93DF-4F84372C110E}"/>
+    <hyperlink ref="L12" r:id="rId2" xr:uid="{98DD1919-A563-7544-91AC-AB29836E3F36}"/>
+    <hyperlink ref="L17" r:id="rId3" display="https://www.digikey.com/product-detail/en/on-semiconductor/FDN337N/FDN337NCT-ND/458950?utm_adgroup=Semiconductor%20Modules&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search&amp;utm_term=&amp;utm_content=Semiconductor%20Modules&amp;gclid=EAIaIQobChMIi9eQ5_aJ6wIViZWzCh0mJgM4EAAYAyAAEgLjm_D_BwE" xr:uid="{727D9452-DCB8-844E-BF89-43B323259E0B}"/>
+    <hyperlink ref="L18" r:id="rId4" xr:uid="{03DCA83F-0C7E-474D-8D58-6E92232C5244}"/>
+    <hyperlink ref="L19" r:id="rId5" xr:uid="{4E66FF84-63D1-5A44-BA0F-60E32688FB28}"/>
+    <hyperlink ref="L31" r:id="rId6" xr:uid="{08520816-E0C6-6E45-BCEA-EBC0C077BDC9}"/>
+    <hyperlink ref="L32" r:id="rId7" xr:uid="{83EC565D-9D7B-DF49-A297-6122E5AA869D}"/>
+    <hyperlink ref="L13" r:id="rId8" xr:uid="{B7D0A652-9B64-FA4C-90B4-EC7144C34A0F}"/>
+    <hyperlink ref="L38" r:id="rId9" xr:uid="{B42B9F1E-03C4-654E-B640-70B7B091A95F}"/>
+    <hyperlink ref="L39" r:id="rId10" xr:uid="{5F7D6664-EBDE-AD43-8A67-C7DC6C8EF2FD}"/>
+    <hyperlink ref="L37" r:id="rId11" xr:uid="{71123794-4398-5A4B-95A8-B03C0806F9B7}"/>
+    <hyperlink ref="L4" r:id="rId12" xr:uid="{8D8D022A-2B79-4B43-AF79-E88260E2C4EB}"/>
+    <hyperlink ref="L11" r:id="rId13" xr:uid="{DD0F3AF5-BF10-2948-9838-14F72CCFC080}"/>
+    <hyperlink ref="L36" r:id="rId14" xr:uid="{763C906E-F39F-B748-9DCE-D60D9F1B5BA1}"/>
+    <hyperlink ref="L28" r:id="rId15" xr:uid="{C31D76A1-733B-B149-9D27-7D33A6F05267}"/>
+    <hyperlink ref="L29" r:id="rId16" xr:uid="{0B9469BA-9B0C-DB44-9532-6B65CA5D2D80}"/>
+    <hyperlink ref="L30" r:id="rId17" xr:uid="{BC8A6AF4-90C7-424F-BEE7-394A1F6FA62B}"/>
+    <hyperlink ref="L5" r:id="rId18" xr:uid="{57D3C9F8-B7A9-0A4E-AB7C-869AD9D6EFEE}"/>
+    <hyperlink ref="L6" r:id="rId19" xr:uid="{00B8C381-F17C-2544-97E4-FDA193DE0C00}"/>
+    <hyperlink ref="L7" r:id="rId20" xr:uid="{68B20804-E11A-3A4D-94F6-E00A01AE1CBA}"/>
+    <hyperlink ref="L8" r:id="rId21" xr:uid="{958DFC3F-79C9-2049-B6D9-E941F4A82470}"/>
+    <hyperlink ref="L3" r:id="rId22" xr:uid="{6B9B3FD9-8979-DF45-9AF2-2185830CDD2D}"/>
+    <hyperlink ref="L21" r:id="rId23" xr:uid="{841B1EE2-C971-4140-AB2C-D17BE6DB3A54}"/>
+    <hyperlink ref="L23" r:id="rId24" xr:uid="{307F796B-E082-774D-8C95-1F7292FA00AA}"/>
+    <hyperlink ref="L25" r:id="rId25" xr:uid="{172AA3A3-05C8-A243-8582-AC79D68B538A}"/>
+    <hyperlink ref="L26" r:id="rId26" xr:uid="{4C3EC69B-4EE1-D340-80A4-28B9D5131D02}"/>
+    <hyperlink ref="L27" r:id="rId27" xr:uid="{4B2FD7B7-81C2-3446-9385-E980FFF07A7E}"/>
+    <hyperlink ref="L34" r:id="rId28" xr:uid="{43E01F73-CC2E-1142-B8D8-A6D76D4576A6}"/>
+    <hyperlink ref="L35" r:id="rId29" xr:uid="{D22264F3-A35B-3642-96CC-BA3FE941B646}"/>
+    <hyperlink ref="L20" r:id="rId30" xr:uid="{16B2B45F-8F65-8F44-B94C-7084F52D1303}"/>
+    <hyperlink ref="L22" r:id="rId31" xr:uid="{E796D191-C601-364D-9975-8C6DCA7B087B}"/>
+    <hyperlink ref="L15" r:id="rId32" xr:uid="{A36BB720-81FE-C546-946E-342DE46F9543}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F16B33-8865-344C-80E0-82EC78AACF85}">
   <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="89" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView topLeftCell="A13" zoomScale="89" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2371,7 +3633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB8D72A-3240-714A-8FB7-32F3483C64DF}">
   <dimension ref="A1:N66"/>
   <sheetViews>
@@ -4084,7 +5346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700EBAD9-5F74-724E-B20F-063A5BC601FD}">
   <dimension ref="A1:L66"/>
   <sheetViews>
@@ -5679,7 +6941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1243D131-AC88-2841-BA58-5847EC392F6F}">
   <dimension ref="A1:T61"/>
   <sheetViews>

</xml_diff>

<commit_message>
added footprints for microphone ckt fix
</commit_message>
<xml_diff>
--- a/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-3.xlsx
+++ b/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2-3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenadachi/Documents/GitHub/pufferfish-electronics/designs/Pufferfish-Interface-2/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16A2F08-96D4-FA40-B0B0-A536FC5EE8B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5878F0-3E89-FF40-BCB3-640FE67E42B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="6340" windowWidth="24000" windowHeight="14500" xr2:uid="{BF342C2E-30CB-B64F-8C68-8C3D8463BC82}"/>
+    <workbookView xWindow="1100" yWindow="460" windowWidth="24000" windowHeight="14500" xr2:uid="{BF342C2E-30CB-B64F-8C68-8C3D8463BC82}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM v2-4" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="233">
   <si>
     <t>Image</t>
   </si>
@@ -730,6 +730,12 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/0908140920/WM3966CT-ND/2421940</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/phoenix-contact/1778719/277-10160-1-ND/5131544</t>
+  </si>
+  <si>
+    <t>Pheonix Contact</t>
   </si>
 </sst>
 </file>
@@ -911,7 +917,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -985,6 +991,7 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1303,7 +1310,7 @@
   <dimension ref="A1:T62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1568,32 +1575,31 @@
       </c>
       <c r="M8" s="42"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="35"/>
-      <c r="B9" s="38" t="s">
+    <row r="9" spans="1:20" s="51" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="50"/>
+      <c r="B9" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="39" t="s">
+      <c r="E9" s="50" t="s">
+        <v>232</v>
+      </c>
+      <c r="F9" s="55">
+        <v>1778719</v>
+      </c>
+      <c r="G9" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="39">
-        <v>1</v>
-      </c>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="40" t="s">
-        <v>178</v>
-      </c>
-      <c r="M9" s="42"/>
+      <c r="H9" s="53">
+        <v>1</v>
+      </c>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="K9" s="50"/>
+      <c r="L9" s="54" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="10" spans="1:20" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="50"/>

</xml_diff>